<commit_message>
[Project] Fixing Bug Hosting
</commit_message>
<xml_diff>
--- a/result-kmeans.xlsx
+++ b/result-kmeans.xlsx
@@ -154,7 +154,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -174,7 +174,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -194,7 +194,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
@@ -214,7 +214,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
@@ -234,7 +234,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" t="s">
         <v>7</v>
@@ -254,7 +254,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="s">
         <v>6</v>
@@ -274,7 +274,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" t="s">
         <v>7</v>
@@ -294,7 +294,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="s">
         <v>6</v>
@@ -314,7 +314,7 @@
         <v>9</v>
       </c>
       <c r="E10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" t="s">
         <v>7</v>
@@ -334,7 +334,7 @@
         <v>10</v>
       </c>
       <c r="E11" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="s">
         <v>6</v>
@@ -354,7 +354,7 @@
         <v>11</v>
       </c>
       <c r="E12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="s">
         <v>7</v>
@@ -374,7 +374,7 @@
         <v>12</v>
       </c>
       <c r="E13" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="s">
         <v>6</v>
@@ -394,7 +394,7 @@
         <v>13</v>
       </c>
       <c r="E14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="s">
         <v>7</v>
@@ -414,7 +414,7 @@
         <v>14</v>
       </c>
       <c r="E15" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" t="s">
         <v>6</v>
@@ -434,7 +434,7 @@
         <v>15</v>
       </c>
       <c r="E16" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" t="s">
         <v>7</v>
@@ -454,7 +454,7 @@
         <v>16</v>
       </c>
       <c r="E17" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="s">
         <v>6</v>
@@ -474,7 +474,7 @@
         <v>17</v>
       </c>
       <c r="E18" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" t="s">
         <v>7</v>
@@ -494,7 +494,7 @@
         <v>18</v>
       </c>
       <c r="E19" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="s">
         <v>6</v>
@@ -514,7 +514,7 @@
         <v>19</v>
       </c>
       <c r="E20" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" t="s">
         <v>7</v>
@@ -534,7 +534,7 @@
         <v>20</v>
       </c>
       <c r="E21" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="s">
         <v>6</v>
@@ -554,7 +554,7 @@
         <v>21</v>
       </c>
       <c r="E22" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" t="s">
         <v>7</v>
@@ -574,7 +574,7 @@
         <v>22</v>
       </c>
       <c r="E23" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="s">
         <v>6</v>
@@ -594,7 +594,7 @@
         <v>23</v>
       </c>
       <c r="E24" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" t="s">
         <v>7</v>
@@ -614,7 +614,7 @@
         <v>24</v>
       </c>
       <c r="E25" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="s">
         <v>6</v>
@@ -634,7 +634,7 @@
         <v>25</v>
       </c>
       <c r="E26" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26" t="s">
         <v>7</v>
@@ -654,7 +654,7 @@
         <v>26</v>
       </c>
       <c r="E27" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="s">
         <v>6</v>
@@ -674,7 +674,7 @@
         <v>27</v>
       </c>
       <c r="E28" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28" t="s">
         <v>7</v>
@@ -694,7 +694,7 @@
         <v>28</v>
       </c>
       <c r="E29" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="s">
         <v>6</v>
@@ -714,7 +714,7 @@
         <v>29</v>
       </c>
       <c r="E30" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30" t="s">
         <v>7</v>
@@ -734,7 +734,7 @@
         <v>30</v>
       </c>
       <c r="E31" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="s">
         <v>6</v>
@@ -754,7 +754,7 @@
         <v>31</v>
       </c>
       <c r="E32" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F32" t="s">
         <v>7</v>
@@ -774,7 +774,7 @@
         <v>32</v>
       </c>
       <c r="E33" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="s">
         <v>6</v>
@@ -794,7 +794,7 @@
         <v>33</v>
       </c>
       <c r="E34" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34" t="s">
         <v>7</v>
@@ -814,7 +814,7 @@
         <v>34</v>
       </c>
       <c r="E35" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="s">
         <v>6</v>
@@ -834,7 +834,7 @@
         <v>35</v>
       </c>
       <c r="E36" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36" t="s">
         <v>7</v>
@@ -854,7 +854,7 @@
         <v>36</v>
       </c>
       <c r="E37" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="s">
         <v>6</v>
@@ -874,7 +874,7 @@
         <v>37</v>
       </c>
       <c r="E38" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38" t="s">
         <v>7</v>
@@ -894,7 +894,7 @@
         <v>38</v>
       </c>
       <c r="E39" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="s">
         <v>6</v>
@@ -914,7 +914,7 @@
         <v>39</v>
       </c>
       <c r="E40" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F40" t="s">
         <v>7</v>
@@ -934,7 +934,7 @@
         <v>40</v>
       </c>
       <c r="E41" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="s">
         <v>6</v>
@@ -954,7 +954,7 @@
         <v>41</v>
       </c>
       <c r="E42" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42" t="s">
         <v>7</v>
@@ -974,7 +974,7 @@
         <v>42</v>
       </c>
       <c r="E43" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="s">
         <v>6</v>
@@ -994,7 +994,7 @@
         <v>43</v>
       </c>
       <c r="E44" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" t="s">
         <v>7</v>
@@ -1014,7 +1014,7 @@
         <v>44</v>
       </c>
       <c r="E45" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="s">
         <v>6</v>
@@ -1034,7 +1034,7 @@
         <v>45</v>
       </c>
       <c r="E46" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46" t="s">
         <v>7</v>
@@ -1054,7 +1054,7 @@
         <v>46</v>
       </c>
       <c r="E47" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="s">
         <v>6</v>
@@ -1074,7 +1074,7 @@
         <v>47</v>
       </c>
       <c r="E48" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48" t="s">
         <v>7</v>
@@ -1094,7 +1094,7 @@
         <v>48</v>
       </c>
       <c r="E49" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F49" t="s">
         <v>8</v>
@@ -1114,7 +1114,7 @@
         <v>49</v>
       </c>
       <c r="E50" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F50" t="s">
         <v>8</v>
@@ -1134,7 +1134,7 @@
         <v>50</v>
       </c>
       <c r="E51" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F51" t="s">
         <v>8</v>
@@ -1154,7 +1154,7 @@
         <v>51</v>
       </c>
       <c r="E52" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F52" t="s">
         <v>7</v>
@@ -1174,7 +1174,7 @@
         <v>52</v>
       </c>
       <c r="E53" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F53" t="s">
         <v>8</v>
@@ -1194,7 +1194,7 @@
         <v>53</v>
       </c>
       <c r="E54" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F54" t="s">
         <v>8</v>
@@ -1214,7 +1214,7 @@
         <v>54</v>
       </c>
       <c r="E55" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F55" t="s">
         <v>7</v>
@@ -1234,7 +1234,7 @@
         <v>55</v>
       </c>
       <c r="E56" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F56" t="s">
         <v>7</v>
@@ -1254,7 +1254,7 @@
         <v>56</v>
       </c>
       <c r="E57" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F57" t="s">
         <v>7</v>
@@ -1274,7 +1274,7 @@
         <v>57</v>
       </c>
       <c r="E58" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F58" t="s">
         <v>7</v>
@@ -1294,7 +1294,7 @@
         <v>58</v>
       </c>
       <c r="E59" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F59" t="s">
         <v>7</v>
@@ -1314,7 +1314,7 @@
         <v>59</v>
       </c>
       <c r="E60" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F60" t="s">
         <v>8</v>
@@ -1334,7 +1334,7 @@
         <v>60</v>
       </c>
       <c r="E61" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F61" t="s">
         <v>7</v>
@@ -1354,7 +1354,7 @@
         <v>61</v>
       </c>
       <c r="E62" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F62" t="s">
         <v>7</v>
@@ -1374,7 +1374,7 @@
         <v>62</v>
       </c>
       <c r="E63" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F63" t="s">
         <v>8</v>
@@ -1394,7 +1394,7 @@
         <v>63</v>
       </c>
       <c r="E64" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F64" t="s">
         <v>7</v>
@@ -1414,7 +1414,7 @@
         <v>64</v>
       </c>
       <c r="E65" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F65" t="s">
         <v>7</v>
@@ -1434,7 +1434,7 @@
         <v>65</v>
       </c>
       <c r="E66" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F66" t="s">
         <v>7</v>
@@ -1454,7 +1454,7 @@
         <v>66</v>
       </c>
       <c r="E67" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F67" t="s">
         <v>8</v>
@@ -1474,7 +1474,7 @@
         <v>67</v>
       </c>
       <c r="E68" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F68" t="s">
         <v>8</v>
@@ -1494,7 +1494,7 @@
         <v>68</v>
       </c>
       <c r="E69" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F69" t="s">
         <v>7</v>
@@ -1514,7 +1514,7 @@
         <v>69</v>
       </c>
       <c r="E70" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F70" t="s">
         <v>8</v>
@@ -1534,7 +1534,7 @@
         <v>70</v>
       </c>
       <c r="E71" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F71" t="s">
         <v>8</v>
@@ -1554,7 +1554,7 @@
         <v>71</v>
       </c>
       <c r="E72" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F72" t="s">
         <v>7</v>
@@ -1574,7 +1574,7 @@
         <v>72</v>
       </c>
       <c r="E73" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F73" t="s">
         <v>7</v>
@@ -1594,7 +1594,7 @@
         <v>73</v>
       </c>
       <c r="E74" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F74" t="s">
         <v>7</v>
@@ -1614,7 +1614,7 @@
         <v>74</v>
       </c>
       <c r="E75" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F75" t="s">
         <v>7</v>
@@ -1634,7 +1634,7 @@
         <v>75</v>
       </c>
       <c r="E76" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F76" t="s">
         <v>7</v>
@@ -1654,7 +1654,7 @@
         <v>76</v>
       </c>
       <c r="E77" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F77" t="s">
         <v>8</v>
@@ -1674,7 +1674,7 @@
         <v>77</v>
       </c>
       <c r="E78" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F78" t="s">
         <v>8</v>
@@ -1694,7 +1694,7 @@
         <v>78</v>
       </c>
       <c r="E79" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F79" t="s">
         <v>8</v>
@@ -1714,7 +1714,7 @@
         <v>79</v>
       </c>
       <c r="E80" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F80" t="s">
         <v>8</v>
@@ -1734,7 +1734,7 @@
         <v>80</v>
       </c>
       <c r="E81" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F81" t="s">
         <v>7</v>
@@ -1754,7 +1754,7 @@
         <v>81</v>
       </c>
       <c r="E82" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F82" t="s">
         <v>7</v>
@@ -1774,7 +1774,7 @@
         <v>82</v>
       </c>
       <c r="E83" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F83" t="s">
         <v>8</v>
@@ -1794,7 +1794,7 @@
         <v>83</v>
       </c>
       <c r="E84" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F84" t="s">
         <v>7</v>
@@ -1814,7 +1814,7 @@
         <v>84</v>
       </c>
       <c r="E85" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F85" t="s">
         <v>8</v>
@@ -1834,7 +1834,7 @@
         <v>85</v>
       </c>
       <c r="E86" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F86" t="s">
         <v>8</v>
@@ -1854,7 +1854,7 @@
         <v>86</v>
       </c>
       <c r="E87" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F87" t="s">
         <v>8</v>
@@ -1874,7 +1874,7 @@
         <v>87</v>
       </c>
       <c r="E88" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F88" t="s">
         <v>8</v>
@@ -1894,7 +1894,7 @@
         <v>88</v>
       </c>
       <c r="E89" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F89" t="s">
         <v>8</v>
@@ -1914,7 +1914,7 @@
         <v>89</v>
       </c>
       <c r="E90" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F90" t="s">
         <v>8</v>
@@ -1934,7 +1934,7 @@
         <v>90</v>
       </c>
       <c r="E91" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F91" t="s">
         <v>8</v>
@@ -1954,7 +1954,7 @@
         <v>91</v>
       </c>
       <c r="E92" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F92" t="s">
         <v>7</v>
@@ -1974,7 +1974,7 @@
         <v>92</v>
       </c>
       <c r="E93" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F93" t="s">
         <v>8</v>
@@ -1994,7 +1994,7 @@
         <v>93</v>
       </c>
       <c r="E94" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F94" t="s">
         <v>8</v>
@@ -2014,7 +2014,7 @@
         <v>94</v>
       </c>
       <c r="E95" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F95" t="s">
         <v>8</v>
@@ -2034,7 +2034,7 @@
         <v>95</v>
       </c>
       <c r="E96" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F96" t="s">
         <v>8</v>
@@ -2054,7 +2054,7 @@
         <v>96</v>
       </c>
       <c r="E97" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F97" t="s">
         <v>8</v>
@@ -2074,7 +2074,7 @@
         <v>97</v>
       </c>
       <c r="E98" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F98" t="s">
         <v>8</v>
@@ -2094,7 +2094,7 @@
         <v>98</v>
       </c>
       <c r="E99" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F99" t="s">
         <v>8</v>
@@ -2114,7 +2114,7 @@
         <v>99</v>
       </c>
       <c r="E100" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F100" t="s">
         <v>8</v>
@@ -2134,7 +2134,7 @@
         <v>100</v>
       </c>
       <c r="E101" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F101" t="s">
         <v>8</v>
@@ -2154,7 +2154,7 @@
         <v>101</v>
       </c>
       <c r="E102" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F102" t="s">
         <v>8</v>
@@ -2174,7 +2174,7 @@
         <v>102</v>
       </c>
       <c r="E103" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F103" t="s">
         <v>8</v>
@@ -2194,7 +2194,7 @@
         <v>103</v>
       </c>
       <c r="E104" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F104" t="s">
         <v>7</v>
@@ -2214,7 +2214,7 @@
         <v>104</v>
       </c>
       <c r="E105" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F105" t="s">
         <v>8</v>
@@ -2234,7 +2234,7 @@
         <v>105</v>
       </c>
       <c r="E106" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F106" t="s">
         <v>8</v>
@@ -2254,7 +2254,7 @@
         <v>106</v>
       </c>
       <c r="E107" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F107" t="s">
         <v>8</v>
@@ -2274,7 +2274,7 @@
         <v>107</v>
       </c>
       <c r="E108" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F108" t="s">
         <v>7</v>
@@ -2294,7 +2294,7 @@
         <v>108</v>
       </c>
       <c r="E109" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F109" t="s">
         <v>8</v>
@@ -2314,7 +2314,7 @@
         <v>109</v>
       </c>
       <c r="E110" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F110" t="s">
         <v>7</v>
@@ -2334,7 +2334,7 @@
         <v>110</v>
       </c>
       <c r="E111" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F111" t="s">
         <v>7</v>
@@ -2354,7 +2354,7 @@
         <v>111</v>
       </c>
       <c r="E112" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F112" t="s">
         <v>7</v>
@@ -2374,7 +2374,7 @@
         <v>112</v>
       </c>
       <c r="E113" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F113" t="s">
         <v>8</v>
@@ -2394,7 +2394,7 @@
         <v>113</v>
       </c>
       <c r="E114" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F114" t="s">
         <v>8</v>
@@ -2414,7 +2414,7 @@
         <v>114</v>
       </c>
       <c r="E115" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F115" t="s">
         <v>8</v>
@@ -2434,7 +2434,7 @@
         <v>115</v>
       </c>
       <c r="E116" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F116" t="s">
         <v>8</v>
@@ -2454,7 +2454,7 @@
         <v>116</v>
       </c>
       <c r="E117" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F117" t="s">
         <v>8</v>
@@ -2474,7 +2474,7 @@
         <v>117</v>
       </c>
       <c r="E118" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F118" t="s">
         <v>7</v>
@@ -2494,7 +2494,7 @@
         <v>118</v>
       </c>
       <c r="E119" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F119" t="s">
         <v>8</v>
@@ -2514,7 +2514,7 @@
         <v>119</v>
       </c>
       <c r="E120" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F120" t="s">
         <v>8</v>
@@ -2534,7 +2534,7 @@
         <v>120</v>
       </c>
       <c r="E121" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F121" t="s">
         <v>8</v>
@@ -2554,7 +2554,7 @@
         <v>121</v>
       </c>
       <c r="E122" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F122" t="s">
         <v>8</v>
@@ -2574,7 +2574,7 @@
         <v>122</v>
       </c>
       <c r="E123" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F123" t="s">
         <v>8</v>
@@ -2594,7 +2594,7 @@
         <v>123</v>
       </c>
       <c r="E124" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F124" t="s">
         <v>8</v>
@@ -2614,7 +2614,7 @@
         <v>124</v>
       </c>
       <c r="E125" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F125" t="s">
         <v>9</v>
@@ -2634,7 +2634,7 @@
         <v>125</v>
       </c>
       <c r="E126" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F126" t="s">
         <v>8</v>
@@ -2654,7 +2654,7 @@
         <v>126</v>
       </c>
       <c r="E127" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F127" t="s">
         <v>9</v>
@@ -2674,7 +2674,7 @@
         <v>127</v>
       </c>
       <c r="E128" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F128" t="s">
         <v>8</v>
@@ -2694,7 +2694,7 @@
         <v>128</v>
       </c>
       <c r="E129" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F129" t="s">
         <v>9</v>
@@ -2734,7 +2734,7 @@
         <v>130</v>
       </c>
       <c r="E131" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F131" t="s">
         <v>9</v>
@@ -2774,7 +2774,7 @@
         <v>132</v>
       </c>
       <c r="E133" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F133" t="s">
         <v>9</v>
@@ -2794,7 +2794,7 @@
         <v>133</v>
       </c>
       <c r="E134" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F134" t="s">
         <v>8</v>
@@ -2814,7 +2814,7 @@
         <v>134</v>
       </c>
       <c r="E135" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F135" t="s">
         <v>9</v>
@@ -2854,7 +2854,7 @@
         <v>136</v>
       </c>
       <c r="E137" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F137" t="s">
         <v>9</v>
@@ -2894,7 +2894,7 @@
         <v>138</v>
       </c>
       <c r="E139" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F139" t="s">
         <v>9</v>
@@ -2934,7 +2934,7 @@
         <v>140</v>
       </c>
       <c r="E141" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F141" t="s">
         <v>9</v>
@@ -2974,7 +2974,7 @@
         <v>142</v>
       </c>
       <c r="E143" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F143" t="s">
         <v>9</v>
@@ -2994,7 +2994,7 @@
         <v>143</v>
       </c>
       <c r="E144" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F144" t="s">
         <v>8</v>
@@ -3014,7 +3014,7 @@
         <v>144</v>
       </c>
       <c r="E145" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F145" t="s">
         <v>9</v>
@@ -3054,7 +3054,7 @@
         <v>146</v>
       </c>
       <c r="E147" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F147" t="s">
         <v>9</v>
@@ -3094,7 +3094,7 @@
         <v>148</v>
       </c>
       <c r="E149" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F149" t="s">
         <v>9</v>
@@ -3134,7 +3134,7 @@
         <v>150</v>
       </c>
       <c r="E151" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F151" t="s">
         <v>9</v>
@@ -3174,7 +3174,7 @@
         <v>152</v>
       </c>
       <c r="E153" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F153" t="s">
         <v>9</v>
@@ -3214,7 +3214,7 @@
         <v>154</v>
       </c>
       <c r="E155" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F155" t="s">
         <v>9</v>
@@ -3254,7 +3254,7 @@
         <v>156</v>
       </c>
       <c r="E157" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F157" t="s">
         <v>9</v>
@@ -3294,7 +3294,7 @@
         <v>158</v>
       </c>
       <c r="E159" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F159" t="s">
         <v>9</v>
@@ -3334,7 +3334,7 @@
         <v>160</v>
       </c>
       <c r="E161" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F161" t="s">
         <v>9</v>
@@ -3374,7 +3374,7 @@
         <v>162</v>
       </c>
       <c r="E163" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F163" t="s">
         <v>9</v>
@@ -3414,7 +3414,7 @@
         <v>164</v>
       </c>
       <c r="E165" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F165" t="s">
         <v>9</v>
@@ -3454,7 +3454,7 @@
         <v>166</v>
       </c>
       <c r="E167" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F167" t="s">
         <v>9</v>
@@ -3494,7 +3494,7 @@
         <v>168</v>
       </c>
       <c r="E169" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F169" t="s">
         <v>9</v>
@@ -3534,7 +3534,7 @@
         <v>170</v>
       </c>
       <c r="E171" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F171" t="s">
         <v>9</v>
@@ -3574,7 +3574,7 @@
         <v>172</v>
       </c>
       <c r="E173" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F173" t="s">
         <v>9</v>
@@ -3614,7 +3614,7 @@
         <v>174</v>
       </c>
       <c r="E175" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F175" t="s">
         <v>9</v>
@@ -3654,7 +3654,7 @@
         <v>176</v>
       </c>
       <c r="E177" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F177" t="s">
         <v>9</v>
@@ -3694,7 +3694,7 @@
         <v>178</v>
       </c>
       <c r="E179" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F179" t="s">
         <v>9</v>
@@ -3734,7 +3734,7 @@
         <v>180</v>
       </c>
       <c r="E181" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F181" t="s">
         <v>9</v>
@@ -3774,7 +3774,7 @@
         <v>182</v>
       </c>
       <c r="E183" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F183" t="s">
         <v>9</v>
@@ -3814,7 +3814,7 @@
         <v>184</v>
       </c>
       <c r="E185" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F185" t="s">
         <v>9</v>
@@ -3854,7 +3854,7 @@
         <v>186</v>
       </c>
       <c r="E187" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F187" t="s">
         <v>9</v>
@@ -3894,7 +3894,7 @@
         <v>188</v>
       </c>
       <c r="E189" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F189" t="s">
         <v>9</v>
@@ -3934,7 +3934,7 @@
         <v>190</v>
       </c>
       <c r="E191" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F191" t="s">
         <v>9</v>
@@ -3974,7 +3974,7 @@
         <v>192</v>
       </c>
       <c r="E193" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F193" t="s">
         <v>9</v>
@@ -4014,7 +4014,7 @@
         <v>194</v>
       </c>
       <c r="E195" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F195" t="s">
         <v>9</v>
@@ -4054,7 +4054,7 @@
         <v>196</v>
       </c>
       <c r="E197" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F197" t="s">
         <v>9</v>
@@ -4094,7 +4094,7 @@
         <v>198</v>
       </c>
       <c r="E199" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F199" t="s">
         <v>9</v>
@@ -4134,7 +4134,7 @@
         <v>200</v>
       </c>
       <c r="E201" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F201" t="s">
         <v>9</v>

</xml_diff>